<commit_message>
Guarda la descripción de la lesion
</commit_message>
<xml_diff>
--- a/media/excel/expedientes.xlsx
+++ b/media/excel/expedientes.xlsx
@@ -505,7 +505,11 @@
           <t>SERIGRAFÍA</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>PRUEBA</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>CUTER</t>
@@ -533,7 +537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -624,7 +628,11 @@
           <t>SERIGRAFÍA</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>PRUEBA</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>MÁQUINA SERIGRAFÍA</t>
@@ -638,6 +646,58 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>ATRAPAMIENTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Accidente con baja</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Publindal</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-11-18</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>MARÍA GONZALEZ ALARCÓN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>SERIGRAFÍA</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>PRUEBA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>MÁQUINA SERIGRAFÍA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>TORAX</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CORTE</t>
         </is>
       </c>
     </row>

</xml_diff>